<commit_message>
creating atom parser spacey script
</commit_message>
<xml_diff>
--- a/true_iref_results.xlsx
+++ b/true_iref_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferlee/Documents/CMU/research/DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6AB7FE-26EF-E049-94E3-D99DCD4A429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5692E63-D308-3242-A972-1C2DB22CE9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="460" windowWidth="24320" windowHeight="16180" xr2:uid="{43A0D98C-1456-D64B-98F7-7A4916103A25}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{43A0D98C-1456-D64B-98F7-7A4916103A25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
   <si>
     <t>concatenation of languages</t>
   </si>
@@ -138,9 +139,6 @@
     <t>(142, 'substring'), (142, 'substring'), (143, 'substring')</t>
   </si>
   <si>
-    <t>(35, 'string'), (38, 'strings'), (42, 'string'), (45, 'strings'), (49, 'strings'), (49, 'strings'), (53, 'string'), (53, 'string'), (69, 'strings'), (91, 'string/word'), (91, 'strings'), (96, 'strings'), (100, 'string'), (114, 'string'), (134, 'string'), (139, 'string'), (139, 'string'), (139, 'strings'), (142, 'string'), (172, 'strings'), (368, 'string'), (368, 'string'), (376, 'string'), (389, 'string'), (472, 'strings'), (472, 'string'), (472, 'string')</t>
-  </si>
-  <si>
     <t>IMPLICIT REFERENCES(line number, phrase)</t>
   </si>
   <si>
@@ -478,6 +476,93 @@
   </si>
   <si>
     <t>383, 'programming languages'</t>
+  </si>
+  <si>
+    <t>(35, 'string')</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (38, 'strings')</t>
+  </si>
+  <si>
+    <t>(42, 'string')</t>
+  </si>
+  <si>
+    <t>(45, 'strings')</t>
+  </si>
+  <si>
+    <t>(49, 'strings')</t>
+  </si>
+  <si>
+    <t>(53, 'string')</t>
+  </si>
+  <si>
+    <t>(69, 'strings')</t>
+  </si>
+  <si>
+    <t>(91, 'string/word')</t>
+  </si>
+  <si>
+    <t>(91, 'strings')</t>
+  </si>
+  <si>
+    <t>(96, 'strings')</t>
+  </si>
+  <si>
+    <t>(100, 'string')</t>
+  </si>
+  <si>
+    <t>(114, 'string')</t>
+  </si>
+  <si>
+    <t>(134, 'string'),</t>
+  </si>
+  <si>
+    <t>(139, 'string')</t>
+  </si>
+  <si>
+    <t>(139, 'strings')</t>
+  </si>
+  <si>
+    <t>(142, 'string')</t>
+  </si>
+  <si>
+    <t>(172, 'strings')</t>
+  </si>
+  <si>
+    <t>(368, 'string')</t>
+  </si>
+  <si>
+    <t>(376, 'string')</t>
+  </si>
+  <si>
+    <t>(389, 'string')</t>
+  </si>
+  <si>
+    <t>(472, 'strings')</t>
+  </si>
+  <si>
+    <t>(472, 'string')</t>
+  </si>
+  <si>
+    <t>false positive</t>
+  </si>
+  <si>
+    <t>(6, finite-length string)</t>
+  </si>
+  <si>
+    <t>(6, related to strings)</t>
+  </si>
+  <si>
+    <t>(6, objects with strings)</t>
+  </si>
+  <si>
+    <t>(383, 'creating a string')</t>
+  </si>
+  <si>
+    <t>false negatives</t>
+  </si>
+  <si>
+    <t>total samples</t>
   </si>
 </sst>
 </file>
@@ -865,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD185ED6-16F1-F249-ACAE-06AB37D1FC2F}">
-  <dimension ref="A1:AQ30"/>
+  <dimension ref="A1:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,10 +978,10 @@
         <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -907,7 +992,7 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -937,10 +1022,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
         <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -962,7 +1047,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -978,7 +1063,7 @@
         <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -999,7 +1084,7 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1010,7 +1095,7 @@
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1031,7 +1116,7 @@
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.2">
@@ -1044,97 +1129,97 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
         <v>121</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>122</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>123</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>124</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>125</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>126</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>127</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
+        <v>127</v>
+      </c>
+      <c r="L20" t="s">
         <v>128</v>
       </c>
-      <c r="K20" t="s">
-        <v>128</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>129</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>130</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>131</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>132</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>133</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>134</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>135</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>136</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
+        <v>136</v>
+      </c>
+      <c r="V20" t="s">
         <v>137</v>
       </c>
-      <c r="U20" t="s">
-        <v>137</v>
-      </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>138</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>139</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>140</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>141</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AA20" t="s">
         <v>142</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AB20" t="s">
         <v>143</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>144</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>145</v>
       </c>
-      <c r="AD20" t="s">
-        <v>146</v>
-      </c>
       <c r="AE20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AF20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AG20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.2">
@@ -1229,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="AG21" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH21" t="s">
         <v>147</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.2">
@@ -1240,124 +1325,121 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>46</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>47</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>48</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" t="s">
         <v>49</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>49</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
+        <v>49</v>
+      </c>
+      <c r="L22" t="s">
         <v>50</v>
       </c>
-      <c r="J22" t="s">
+      <c r="M22" t="s">
         <v>50</v>
       </c>
-      <c r="K22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>51</v>
       </c>
-      <c r="M22" t="s">
-        <v>51</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>52</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>53</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
+        <v>55</v>
+      </c>
+      <c r="R22" t="s">
         <v>54</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="S22" t="s">
+        <v>54</v>
+      </c>
+      <c r="T22" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22" t="s">
+        <v>55</v>
+      </c>
+      <c r="V22" t="s">
         <v>56</v>
       </c>
-      <c r="R22" t="s">
-        <v>55</v>
-      </c>
-      <c r="S22" t="s">
-        <v>55</v>
-      </c>
-      <c r="T22" t="s">
-        <v>56</v>
-      </c>
-      <c r="U22" t="s">
-        <v>56</v>
-      </c>
-      <c r="V22" t="s">
+      <c r="W22" t="s">
+        <v>54</v>
+      </c>
+      <c r="X22" t="s">
         <v>57</v>
       </c>
-      <c r="W22" t="s">
-        <v>55</v>
-      </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>58</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>59</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>60</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>61</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD22" t="s">
         <v>62</v>
       </c>
-      <c r="AC22" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>63</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AF22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AF22" s="5" t="s">
+      <c r="AG22" t="s">
         <v>65</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AH22" t="s">
         <v>66</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AI22" t="s">
         <v>67</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AJ22" t="s">
         <v>68</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AK22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL22" t="s">
         <v>69</v>
       </c>
-      <c r="AK22" t="s">
+      <c r="AM22" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN22" t="s">
         <v>71</v>
       </c>
-      <c r="AL22" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM22" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN22" t="s">
-        <v>72</v>
-      </c>
       <c r="AO22" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.2">
@@ -1479,10 +1561,10 @@
         <v>1</v>
       </c>
       <c r="AP23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AQ23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
@@ -1490,106 +1572,106 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
         <v>93</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>94</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>95</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>96</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>97</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>98</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>99</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>100</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>101</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>102</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>103</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>104</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>105</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>106</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>107</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>108</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>109</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>110</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>111</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
+        <v>111</v>
+      </c>
+      <c r="X24" t="s">
         <v>112</v>
       </c>
-      <c r="W24" t="s">
+      <c r="Y24" t="s">
         <v>112</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Z24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB24" t="s">
         <v>113</v>
       </c>
-      <c r="Y24" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB24" t="s">
+      <c r="AC24" t="s">
         <v>114</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AD24" t="s">
         <v>115</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>116</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AF24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG24" t="s">
         <v>117</v>
       </c>
-      <c r="AF24" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG24" t="s">
+      <c r="AH24" t="s">
         <v>118</v>
       </c>
-      <c r="AH24" t="s">
+      <c r="AI24" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ24" t="s">
         <v>119</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.2">
@@ -1701,67 +1783,67 @@
         <v>19</v>
       </c>
       <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" t="s">
         <v>75</v>
       </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>76</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>77</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>78</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>79</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>80</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>81</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>82</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>83</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>84</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>85</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>86</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
+        <v>86</v>
+      </c>
+      <c r="R26" t="s">
+        <v>86</v>
+      </c>
+      <c r="S26" t="s">
         <v>87</v>
       </c>
-      <c r="Q26" t="s">
-        <v>87</v>
-      </c>
-      <c r="R26" t="s">
-        <v>87</v>
-      </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>88</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
+        <v>91</v>
+      </c>
+      <c r="V26" t="s">
         <v>89</v>
       </c>
-      <c r="U26" t="s">
-        <v>92</v>
-      </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>90</v>
-      </c>
-      <c r="W26" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.2">
@@ -1834,12 +1916,266 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>148</v>
+      </c>
+      <c r="D28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" t="s">
+        <v>151</v>
+      </c>
+      <c r="G28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" t="s">
+        <v>152</v>
+      </c>
+      <c r="I28" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K28" t="s">
+        <v>154</v>
+      </c>
+      <c r="L28" t="s">
+        <v>155</v>
+      </c>
+      <c r="M28" t="s">
+        <v>156</v>
+      </c>
+      <c r="N28" t="s">
+        <v>157</v>
+      </c>
+      <c r="O28" t="s">
+        <v>158</v>
+      </c>
+      <c r="P28" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>160</v>
+      </c>
+      <c r="R28" t="s">
+        <v>161</v>
+      </c>
+      <c r="S28" t="s">
+        <v>161</v>
+      </c>
+      <c r="T28" t="s">
+        <v>162</v>
+      </c>
+      <c r="U28" t="s">
+        <v>163</v>
+      </c>
+      <c r="V28" t="s">
+        <v>164</v>
+      </c>
+      <c r="W28" t="s">
+        <v>165</v>
+      </c>
+      <c r="X28" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <f>D35/D37*100</f>
+        <v>2.6595744680851063</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36">
+        <f>15+13+2</f>
+        <v>30</v>
+      </c>
+      <c r="E36">
+        <f>D36/D37*100</f>
+        <v>15.957446808510639</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37">
+        <f>12+9+15+30+39+34+21+28</f>
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E1DE4C-0C59-6C45-8625-2C84244940A9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>